<commit_message>
removed a blank line in the chelyabinsk lcs since it was messing with the integrated intensity calculations
</commit_message>
<xml_diff>
--- a/speed_radiant_difference/events/Chelyabinsk/chelyabinsk_lc_INT.xlsx
+++ b/speed_radiant_difference/events/Chelyabinsk/chelyabinsk_lc_INT.xlsx
@@ -121,10 +121,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B341"/>
+  <dimension ref="A1:B340"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A163" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F182" activeCellId="0" sqref="F182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1572,1283 +1572,1283 @@
         <v>27289777828.0804</v>
       </c>
     </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="1" t="n">
+        <v>-3.5703</v>
+      </c>
+      <c r="B181" s="0" t="n">
+        <v>42344791616.9207</v>
+      </c>
+    </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="n">
-        <v>-3.5703</v>
+        <v>-3.5369</v>
       </c>
       <c r="B182" s="0" t="n">
-        <v>42344791616.9207</v>
+        <v>42997182672.3838</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="n">
-        <v>-3.5369</v>
+        <v>-3.5035</v>
       </c>
       <c r="B183" s="0" t="n">
-        <v>42997182672.3838</v>
+        <v>44471317911.9487</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="n">
-        <v>-3.5035</v>
+        <v>-3.4702</v>
       </c>
       <c r="B184" s="0" t="n">
-        <v>44471317911.9487</v>
+        <v>44738353832.7868</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="n">
-        <v>-3.4702</v>
+        <v>-3.4368</v>
       </c>
       <c r="B185" s="0" t="n">
-        <v>44738353832.7868</v>
+        <v>42981344842.5012</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="n">
-        <v>-3.4368</v>
+        <v>-3.4034</v>
       </c>
       <c r="B186" s="0" t="n">
-        <v>42981344842.5012</v>
+        <v>43639523512.026</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="n">
-        <v>-3.4034</v>
+        <v>-3.3701</v>
       </c>
       <c r="B187" s="0" t="n">
-        <v>43639523512.026</v>
+        <v>45127367527.1812</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="n">
-        <v>-3.3701</v>
+        <v>-3.3367</v>
       </c>
       <c r="B188" s="0" t="n">
-        <v>45127367527.1812</v>
+        <v>43207585698.0492</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="n">
-        <v>-3.3367</v>
+        <v>-3.3033</v>
       </c>
       <c r="B189" s="0" t="n">
-        <v>43207585698.0492</v>
+        <v>45094128701.1199</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="n">
-        <v>-3.3033</v>
+        <v>-3.27</v>
       </c>
       <c r="B190" s="0" t="n">
-        <v>45094128701.1199</v>
+        <v>47058708062.911</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="n">
-        <v>-3.27</v>
+        <v>-3.2366</v>
       </c>
       <c r="B191" s="0" t="n">
-        <v>47058708062.911</v>
+        <v>50021878844.6234</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="n">
-        <v>-3.2366</v>
+        <v>-3.2032</v>
       </c>
       <c r="B192" s="0" t="n">
-        <v>50021878844.6234</v>
+        <v>48493105808.3615</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="n">
-        <v>-3.2032</v>
+        <v>-3.1699</v>
       </c>
       <c r="B193" s="0" t="n">
-        <v>48493105808.3615</v>
+        <v>54470329198.9893</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="n">
-        <v>-3.1699</v>
+        <v>-3.1365</v>
       </c>
       <c r="B194" s="0" t="n">
-        <v>54470329198.9893</v>
+        <v>53599408866.2705</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="n">
-        <v>-3.1365</v>
+        <v>-3.1031</v>
       </c>
       <c r="B195" s="0" t="n">
-        <v>53599408866.2705</v>
+        <v>53713073039.4835</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="n">
-        <v>-3.1031</v>
+        <v>-3.0698</v>
       </c>
       <c r="B196" s="0" t="n">
-        <v>53713073039.4835</v>
+        <v>55019925753.9476</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="n">
-        <v>-3.0698</v>
+        <v>-3.0364</v>
       </c>
       <c r="B197" s="0" t="n">
-        <v>55019925753.9476</v>
+        <v>59560728354.4559</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="n">
-        <v>-3.0364</v>
+        <v>-3.003</v>
       </c>
       <c r="B198" s="0" t="n">
-        <v>59560728354.4559</v>
+        <v>57200523041.5929</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="n">
-        <v>-3.003</v>
+        <v>-2.9697</v>
       </c>
       <c r="B199" s="0" t="n">
-        <v>57200523041.5929</v>
+        <v>57846887987.5293</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="n">
-        <v>-2.9697</v>
+        <v>-2.9363</v>
       </c>
       <c r="B200" s="0" t="n">
-        <v>57846887987.5293</v>
+        <v>63779336949.2826</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="n">
-        <v>-2.9363</v>
+        <v>-2.9029</v>
       </c>
       <c r="B201" s="0" t="n">
-        <v>63779336949.2826</v>
+        <v>65935605688.7909</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="n">
-        <v>-2.9029</v>
+        <v>-2.8696</v>
       </c>
       <c r="B202" s="0" t="n">
-        <v>65935605688.7909</v>
+        <v>64851496167.4144</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="n">
-        <v>-2.8696</v>
+        <v>-2.8362</v>
       </c>
       <c r="B203" s="0" t="n">
-        <v>64851496167.4144</v>
+        <v>72163900660.7037</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="n">
-        <v>-2.8362</v>
+        <v>-2.8028</v>
       </c>
       <c r="B204" s="0" t="n">
-        <v>72163900660.7037</v>
+        <v>73912858759.7937</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="n">
-        <v>-2.8028</v>
+        <v>-2.7695</v>
       </c>
       <c r="B205" s="0" t="n">
-        <v>73912858759.7937</v>
+        <v>74741188582.6742</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="n">
-        <v>-2.7695</v>
+        <v>-2.7361</v>
       </c>
       <c r="B206" s="0" t="n">
-        <v>74741188582.6742</v>
+        <v>80902138212.3821</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="n">
-        <v>-2.7361</v>
+        <v>-2.7027</v>
       </c>
       <c r="B207" s="0" t="n">
-        <v>80902138212.3821</v>
+        <v>91698028821.9735</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="n">
-        <v>-2.7027</v>
+        <v>-2.6694</v>
       </c>
       <c r="B208" s="0" t="n">
-        <v>91698028821.9735</v>
+        <v>96551716702.8731</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="n">
-        <v>-2.6694</v>
+        <v>-2.636</v>
       </c>
       <c r="B209" s="0" t="n">
-        <v>96551716702.8731</v>
+        <v>101288467433.772</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="n">
-        <v>-2.636</v>
+        <v>-2.6026</v>
       </c>
       <c r="B210" s="0" t="n">
-        <v>101288467433.772</v>
+        <v>103752841581.801</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="n">
-        <v>-2.6026</v>
+        <v>-2.5693</v>
       </c>
       <c r="B211" s="0" t="n">
-        <v>103752841581.801</v>
+        <v>116519872302.5</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="n">
-        <v>-2.5693</v>
+        <v>-2.5359</v>
       </c>
       <c r="B212" s="0" t="n">
-        <v>116519872302.5</v>
+        <v>147516296303.296</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="n">
-        <v>-2.5359</v>
+        <v>-2.5025</v>
       </c>
       <c r="B213" s="0" t="n">
-        <v>147516296303.296</v>
+        <v>168764073690.718</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="n">
-        <v>-2.5025</v>
+        <v>-2.4692</v>
       </c>
       <c r="B214" s="0" t="n">
-        <v>168764073690.718</v>
+        <v>166617264498.612</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="n">
-        <v>-2.4692</v>
+        <v>-2.4358</v>
       </c>
       <c r="B215" s="0" t="n">
-        <v>166617264498.612</v>
+        <v>170671104877.964</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="n">
-        <v>-2.4358</v>
+        <v>-2.4024</v>
       </c>
       <c r="B216" s="0" t="n">
-        <v>170671104877.964</v>
+        <v>186483323257.71</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="n">
-        <v>-2.4024</v>
+        <v>-2.3691</v>
       </c>
       <c r="B217" s="0" t="n">
-        <v>186483323257.71</v>
+        <v>193909907861.485</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="n">
-        <v>-2.3691</v>
+        <v>-2.3357</v>
       </c>
       <c r="B218" s="0" t="n">
-        <v>193909907861.485</v>
+        <v>241034939056.099</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="n">
-        <v>-2.3357</v>
+        <v>-2.3023</v>
       </c>
       <c r="B219" s="0" t="n">
-        <v>241034939056.099</v>
+        <v>251535912916.328</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="1" t="n">
-        <v>-2.3023</v>
+        <v>-2.269</v>
       </c>
       <c r="B220" s="0" t="n">
-        <v>251535912916.328</v>
+        <v>289547620329.64</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="n">
-        <v>-2.269</v>
+        <v>-2.2356</v>
       </c>
       <c r="B221" s="0" t="n">
-        <v>289547620329.64</v>
+        <v>316431711329.18</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="n">
-        <v>-2.2356</v>
+        <v>-2.2022</v>
       </c>
       <c r="B222" s="0" t="n">
-        <v>316431711329.18</v>
+        <v>339531443623.172</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="1" t="n">
-        <v>-2.2022</v>
+        <v>-2.1689</v>
       </c>
       <c r="B223" s="0" t="n">
-        <v>339531443623.172</v>
+        <v>341601681662.632</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="1" t="n">
-        <v>-2.1689</v>
+        <v>-2.1355</v>
       </c>
       <c r="B224" s="0" t="n">
-        <v>341601681662.632</v>
+        <v>353313311251.725</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="1" t="n">
-        <v>-2.1355</v>
+        <v>-2.1021</v>
       </c>
       <c r="B225" s="0" t="n">
-        <v>353313311251.725</v>
+        <v>358756683039.262</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="1" t="n">
-        <v>-2.1021</v>
+        <v>-2.0688</v>
       </c>
       <c r="B226" s="0" t="n">
-        <v>358756683039.262</v>
+        <v>357700872931.138</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="1" t="n">
-        <v>-2.0688</v>
+        <v>-2.0354</v>
       </c>
       <c r="B227" s="0" t="n">
-        <v>357700872931.138</v>
+        <v>380399554808.905</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="1" t="n">
-        <v>-2.0354</v>
+        <v>-2.002</v>
       </c>
       <c r="B228" s="0" t="n">
-        <v>380399554808.905</v>
+        <v>375837404288.444</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="1" t="n">
-        <v>-2.002</v>
+        <v>-1.9687</v>
       </c>
       <c r="B229" s="0" t="n">
-        <v>375837404288.444</v>
+        <v>381768419497.544</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="n">
-        <v>-1.9687</v>
+        <v>-1.9353</v>
       </c>
       <c r="B230" s="0" t="n">
-        <v>381768419497.544</v>
+        <v>347216216172.221</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="n">
-        <v>-1.9353</v>
+        <v>-1.9019</v>
       </c>
       <c r="B231" s="0" t="n">
-        <v>347216216172.221</v>
+        <v>352760541021.545</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="1" t="n">
-        <v>-1.9019</v>
+        <v>-1.8686</v>
       </c>
       <c r="B232" s="0" t="n">
-        <v>352760541021.545</v>
+        <v>315064883297.239</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="n">
-        <v>-1.8686</v>
+        <v>-1.8352</v>
       </c>
       <c r="B233" s="0" t="n">
-        <v>315064883297.239</v>
+        <v>305717289176.049</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="1" t="n">
-        <v>-1.8352</v>
+        <v>-1.8018</v>
       </c>
       <c r="B234" s="0" t="n">
-        <v>305717289176.049</v>
+        <v>302189938301.443</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="n">
-        <v>-1.8018</v>
+        <v>-1.7685</v>
       </c>
       <c r="B235" s="0" t="n">
-        <v>302189938301.443</v>
+        <v>304312645823.863</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="n">
-        <v>-1.7685</v>
+        <v>-1.7351</v>
       </c>
       <c r="B236" s="0" t="n">
-        <v>304312645823.863</v>
+        <v>312176351084.817</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="n">
-        <v>-1.7351</v>
+        <v>-1.7017</v>
       </c>
       <c r="B237" s="0" t="n">
-        <v>312176351084.817</v>
+        <v>351172096216.597</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="n">
-        <v>-1.7017</v>
+        <v>-1.6684</v>
       </c>
       <c r="B238" s="0" t="n">
-        <v>351172096216.597</v>
+        <v>367011776575.004</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="1" t="n">
-        <v>-1.6684</v>
+        <v>-1.635</v>
       </c>
       <c r="B239" s="0" t="n">
-        <v>367011776575.004</v>
+        <v>383636570515.202</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="1" t="n">
-        <v>-1.635</v>
+        <v>-1.6016</v>
       </c>
       <c r="B240" s="0" t="n">
-        <v>383636570515.202</v>
+        <v>439744078447.369</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="n">
-        <v>-1.6016</v>
+        <v>-1.5683</v>
       </c>
       <c r="B241" s="0" t="n">
-        <v>439744078447.369</v>
+        <v>537724717405.866</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="1" t="n">
-        <v>-1.5683</v>
+        <v>-1.5349</v>
       </c>
       <c r="B242" s="0" t="n">
-        <v>537724717405.866</v>
+        <v>682275851319.515</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="1" t="n">
-        <v>-1.5349</v>
+        <v>-1.5015</v>
       </c>
       <c r="B243" s="0" t="n">
-        <v>682275851319.515</v>
+        <v>994031163465.779</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="n">
-        <v>-1.5015</v>
+        <v>-1.4682</v>
       </c>
       <c r="B244" s="0" t="n">
-        <v>994031163465.779</v>
+        <v>1370629263668.38</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="n">
-        <v>-1.4682</v>
+        <v>-1.4348</v>
       </c>
       <c r="B245" s="0" t="n">
-        <v>1370629263668.38</v>
+        <v>1474076423138.71</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="n">
-        <v>-1.4348</v>
+        <v>-1.4014</v>
       </c>
       <c r="B246" s="0" t="n">
-        <v>1474076423138.71</v>
+        <v>1614953418068.88</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="n">
-        <v>-1.4014</v>
+        <v>-1.3681</v>
       </c>
       <c r="B247" s="0" t="n">
-        <v>1614953418068.88</v>
+        <v>2376402496787.06</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="n">
-        <v>-1.3681</v>
+        <v>-1.3347</v>
       </c>
       <c r="B248" s="0" t="n">
-        <v>2376402496787.06</v>
+        <v>2441855722519.2</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="1" t="n">
-        <v>-1.3347</v>
+        <v>-1.3013</v>
       </c>
       <c r="B249" s="0" t="n">
-        <v>2441855722519.2</v>
+        <v>2418577453673.44</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="1" t="n">
-        <v>-1.3013</v>
+        <v>-1.268</v>
       </c>
       <c r="B250" s="0" t="n">
-        <v>2418577453673.44</v>
+        <v>2418800223147.84</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="1" t="n">
-        <v>-1.268</v>
+        <v>-1.2346</v>
       </c>
       <c r="B251" s="0" t="n">
-        <v>2418800223147.84</v>
+        <v>2533494699441.49</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="1" t="n">
-        <v>-1.2346</v>
+        <v>-1.2012</v>
       </c>
       <c r="B252" s="0" t="n">
-        <v>2533494699441.49</v>
+        <v>2536529981524.26</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="1" t="n">
-        <v>-1.2012</v>
+        <v>-1.1679</v>
       </c>
       <c r="B253" s="0" t="n">
-        <v>2536529981524.26</v>
+        <v>2861804748801.32</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="1" t="n">
-        <v>-1.1679</v>
+        <v>-1.1345</v>
       </c>
       <c r="B254" s="0" t="n">
-        <v>2861804748801.32</v>
+        <v>3200073843319.8</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="1" t="n">
-        <v>-1.1345</v>
+        <v>-1.1011</v>
       </c>
       <c r="B255" s="0" t="n">
-        <v>3200073843319.8</v>
+        <v>4342301753641.61</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="1" t="n">
-        <v>-1.1011</v>
+        <v>-1.0678</v>
       </c>
       <c r="B256" s="0" t="n">
-        <v>4342301753641.61</v>
+        <v>5229257163338.77</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="1" t="n">
-        <v>-1.0678</v>
+        <v>-1.0344</v>
       </c>
       <c r="B257" s="0" t="n">
-        <v>5229257163338.77</v>
+        <v>5286886658508.81</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="1" t="n">
-        <v>-1.0344</v>
+        <v>-1.001</v>
       </c>
       <c r="B258" s="0" t="n">
-        <v>5286886658508.81</v>
+        <v>7048878097610.31</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="1" t="n">
-        <v>-1.001</v>
+        <v>-0.9677</v>
       </c>
       <c r="B259" s="0" t="n">
-        <v>7048878097610.31</v>
+        <v>7535637523296.03</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="1" t="n">
-        <v>-0.9677</v>
+        <v>-0.9343</v>
       </c>
       <c r="B260" s="0" t="n">
-        <v>7535637523296.03</v>
+        <v>8594883611113.73</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="n">
-        <v>-0.9343</v>
+        <v>-0.9009</v>
       </c>
       <c r="B261" s="0" t="n">
-        <v>8594883611113.73</v>
+        <v>9805731562195.36</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="n">
-        <v>-0.9009</v>
+        <v>-0.8676</v>
       </c>
       <c r="B262" s="0" t="n">
-        <v>9805731562195.36</v>
+        <v>10685626745999.6</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="1" t="n">
-        <v>-0.8676</v>
+        <v>-0.8342</v>
       </c>
       <c r="B263" s="0" t="n">
-        <v>10685626745999.6</v>
+        <v>10722103620102</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="1" t="n">
-        <v>-0.8342</v>
+        <v>-0.8008</v>
       </c>
       <c r="B264" s="0" t="n">
-        <v>10722103620102</v>
+        <v>11267822577730.6</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="n">
-        <v>-0.8008</v>
+        <v>-0.7675</v>
       </c>
       <c r="B265" s="0" t="n">
-        <v>11267822577730.6</v>
+        <v>13600660503742.2</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="n">
-        <v>-0.7675</v>
+        <v>-0.7341</v>
       </c>
       <c r="B266" s="0" t="n">
-        <v>13600660503742.2</v>
+        <v>13912334146288.1</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="1" t="n">
-        <v>-0.7341</v>
+        <v>-0.7007</v>
       </c>
       <c r="B267" s="0" t="n">
-        <v>13912334146288.1</v>
+        <v>13847137350003.4</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="n">
-        <v>-0.7007</v>
+        <v>-0.6674</v>
       </c>
       <c r="B268" s="0" t="n">
-        <v>13847137350003.4</v>
+        <v>14840208408453.4</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="1" t="n">
-        <v>-0.6674</v>
+        <v>-0.634</v>
       </c>
       <c r="B269" s="0" t="n">
-        <v>14840208408453.4</v>
+        <v>16814346776652.6</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="1" t="n">
-        <v>-0.634</v>
+        <v>-0.6006</v>
       </c>
       <c r="B270" s="0" t="n">
-        <v>16814346776652.6</v>
+        <v>18879913490962.9</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="1" t="n">
-        <v>-0.6006</v>
+        <v>-0.5673</v>
       </c>
       <c r="B271" s="0" t="n">
-        <v>18879913490962.9</v>
+        <v>21208990618524.3</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="n">
-        <v>-0.5673</v>
+        <v>-0.5339</v>
       </c>
       <c r="B272" s="0" t="n">
-        <v>21208990618524.3</v>
+        <v>22137062947618.8</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="1" t="n">
-        <v>-0.5339</v>
+        <v>-0.5005</v>
       </c>
       <c r="B273" s="0" t="n">
-        <v>22137062947618.8</v>
+        <v>23330282630082.4</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="1" t="n">
-        <v>-0.5005</v>
+        <v>-0.4672</v>
       </c>
       <c r="B274" s="0" t="n">
-        <v>23330282630082.4</v>
+        <v>24369128610927.7</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="n">
-        <v>-0.4672</v>
+        <v>-0.4338</v>
       </c>
       <c r="B275" s="0" t="n">
-        <v>24369128610927.7</v>
+        <v>26174596774555.7</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="n">
-        <v>-0.4338</v>
+        <v>-0.4004</v>
       </c>
       <c r="B276" s="0" t="n">
-        <v>26174596774555.7</v>
+        <v>28124188493835.8</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="n">
-        <v>-0.4004</v>
+        <v>-0.3671</v>
       </c>
       <c r="B277" s="0" t="n">
-        <v>28124188493835.8</v>
+        <v>29678366933469.3</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="n">
-        <v>-0.3671</v>
+        <v>-0.3337</v>
       </c>
       <c r="B278" s="0" t="n">
-        <v>29678366933469.3</v>
+        <v>32502741960736</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="n">
-        <v>-0.3337</v>
+        <v>-0.3003</v>
       </c>
       <c r="B279" s="0" t="n">
-        <v>32502741960736</v>
+        <v>33079581003253.9</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="n">
-        <v>-0.3003</v>
+        <v>-0.267</v>
       </c>
       <c r="B280" s="0" t="n">
-        <v>33079581003253.9</v>
+        <v>33987560995553.4</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="1" t="n">
-        <v>-0.267</v>
+        <v>-0.2336</v>
       </c>
       <c r="B281" s="0" t="n">
-        <v>33987560995553.4</v>
+        <v>34311523340052.9</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="1" t="n">
-        <v>-0.2336</v>
+        <v>-0.2002</v>
       </c>
       <c r="B282" s="0" t="n">
-        <v>34311523340052.9</v>
+        <v>35948435968227.3</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="1" t="n">
-        <v>-0.2002</v>
+        <v>-0.1669</v>
       </c>
       <c r="B283" s="0" t="n">
-        <v>35948435968227.3</v>
+        <v>36650508116097.4</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="1" t="n">
-        <v>-0.1669</v>
+        <v>-0.1335</v>
       </c>
       <c r="B284" s="0" t="n">
-        <v>36650508116097.4</v>
+        <v>37729408792345.7</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="n">
-        <v>-0.1335</v>
+        <v>-0.1001</v>
       </c>
       <c r="B285" s="0" t="n">
-        <v>37729408792345.7</v>
+        <v>38494616734245</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="1" t="n">
-        <v>-0.1001</v>
+        <v>-0.0668</v>
       </c>
       <c r="B286" s="0" t="n">
-        <v>38494616734245</v>
+        <v>39289816456729.4</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="1" t="n">
-        <v>-0.0668</v>
+        <v>-0.0334</v>
       </c>
       <c r="B287" s="0" t="n">
-        <v>39289816456729.4</v>
+        <v>39748431886550.5</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="1" t="n">
-        <v>-0.0334</v>
+      <c r="A288" s="2" t="n">
+        <v>-2.9E-005</v>
       </c>
       <c r="B288" s="0" t="n">
-        <v>39748431886550.5</v>
+        <v>39858412736815.6</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="2" t="n">
-        <v>-2.9E-005</v>
+      <c r="A289" s="1" t="n">
+        <v>0.0333</v>
       </c>
       <c r="B289" s="0" t="n">
-        <v>39858412736815.6</v>
+        <v>38183875031679.2</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="1" t="n">
-        <v>0.0333</v>
+        <v>0.0667</v>
       </c>
       <c r="B290" s="0" t="n">
-        <v>38183875031679.2</v>
+        <v>36931759604798.7</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="n">
-        <v>0.0667</v>
+        <v>0.1001</v>
       </c>
       <c r="B291" s="0" t="n">
-        <v>36931759604798.7</v>
+        <v>33502714775537.4</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="1" t="n">
-        <v>0.1001</v>
+        <v>0.1334</v>
       </c>
       <c r="B292" s="0" t="n">
-        <v>33502714775537.4</v>
+        <v>31541329838079.3</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="1" t="n">
-        <v>0.1334</v>
+        <v>0.1668</v>
       </c>
       <c r="B293" s="0" t="n">
-        <v>31541329838079.3</v>
+        <v>31396410591295.5</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="1" t="n">
-        <v>0.1668</v>
+        <v>0.2002</v>
       </c>
       <c r="B294" s="0" t="n">
-        <v>31396410591295.5</v>
+        <v>29856575954815.2</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="1" t="n">
-        <v>0.2002</v>
+        <v>0.2335</v>
       </c>
       <c r="B295" s="0" t="n">
-        <v>29856575954815.2</v>
+        <v>27375370143415.9</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="1" t="n">
-        <v>0.2335</v>
+        <v>0.2669</v>
       </c>
       <c r="B296" s="0" t="n">
-        <v>27375370143415.9</v>
+        <v>26533833523823.4</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="1" t="n">
-        <v>0.2669</v>
+        <v>0.3003</v>
       </c>
       <c r="B297" s="0" t="n">
-        <v>26533833523823.4</v>
+        <v>23680997938737.9</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="1" t="n">
-        <v>0.3003</v>
+        <v>0.3336</v>
       </c>
       <c r="B298" s="0" t="n">
-        <v>23680997938737.9</v>
+        <v>19462561593612.4</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="n">
-        <v>0.3336</v>
+        <v>0.367</v>
       </c>
       <c r="B299" s="0" t="n">
-        <v>19462561593612.4</v>
+        <v>17705981250752.4</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="1" t="n">
-        <v>0.367</v>
+        <v>0.4004</v>
       </c>
       <c r="B300" s="0" t="n">
-        <v>17705981250752.4</v>
+        <v>15388631498199.6</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="1" t="n">
-        <v>0.4004</v>
+        <v>0.4337</v>
       </c>
       <c r="B301" s="0" t="n">
-        <v>15388631498199.6</v>
+        <v>13881615150799.5</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="1" t="n">
-        <v>0.4337</v>
+        <v>0.4671</v>
       </c>
       <c r="B302" s="0" t="n">
-        <v>13881615150799.5</v>
+        <v>11529221952567.7</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="1" t="n">
-        <v>0.4671</v>
+        <v>0.5005</v>
       </c>
       <c r="B303" s="0" t="n">
-        <v>11529221952567.7</v>
+        <v>8899385094848.99</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="1" t="n">
-        <v>0.5005</v>
+        <v>0.5338</v>
       </c>
       <c r="B304" s="0" t="n">
-        <v>8899385094848.99</v>
+        <v>6999064568006.57</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="1" t="n">
-        <v>0.5338</v>
+        <v>0.5672</v>
       </c>
       <c r="B305" s="0" t="n">
-        <v>6999064568006.57</v>
+        <v>5927615158904.13</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="1" t="n">
-        <v>0.5672</v>
+        <v>0.6006</v>
       </c>
       <c r="B306" s="0" t="n">
-        <v>5927615158904.13</v>
+        <v>3915975806487.59</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="1" t="n">
-        <v>0.6006</v>
+        <v>0.6339</v>
       </c>
       <c r="B307" s="0" t="n">
-        <v>3915975806487.59</v>
+        <v>2811641856687.9</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="1" t="n">
-        <v>0.6339</v>
+        <v>0.6673</v>
       </c>
       <c r="B308" s="0" t="n">
-        <v>2811641856687.9</v>
+        <v>2450417018235.52</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="1" t="n">
-        <v>0.6673</v>
+        <v>0.7007</v>
       </c>
       <c r="B309" s="0" t="n">
-        <v>2450417018235.52</v>
+        <v>2175905349985.84</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="1" t="n">
-        <v>0.7007</v>
+        <v>0.734</v>
       </c>
       <c r="B310" s="0" t="n">
-        <v>2175905349985.84</v>
+        <v>1845865275851.3</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="1" t="n">
-        <v>0.734</v>
+        <v>0.7674</v>
       </c>
       <c r="B311" s="0" t="n">
-        <v>1845865275851.3</v>
+        <v>1093754870621.39</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="1" t="n">
-        <v>0.7674</v>
+        <v>0.8008</v>
       </c>
       <c r="B312" s="0" t="n">
-        <v>1093754870621.39</v>
+        <v>1096478196143.19</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="1" t="n">
-        <v>0.8008</v>
+        <v>0.8341</v>
       </c>
       <c r="B313" s="0" t="n">
-        <v>1096478196143.19</v>
+        <v>1116863247780.56</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="1" t="n">
-        <v>0.8341</v>
+        <v>0.8675</v>
       </c>
       <c r="B314" s="0" t="n">
-        <v>1116863247780.56</v>
+        <v>1158777356155.13</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="1" t="n">
-        <v>0.8675</v>
+        <v>0.9009</v>
       </c>
       <c r="B315" s="0" t="n">
-        <v>1158777356155.13</v>
+        <v>1393156802945.3</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="1" t="n">
-        <v>0.9009</v>
+        <v>0.9342</v>
       </c>
       <c r="B316" s="0" t="n">
-        <v>1393156802945.3</v>
+        <v>1513561248436.21</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="1" t="n">
-        <v>0.9342</v>
+        <v>0.9676</v>
       </c>
       <c r="B317" s="0" t="n">
-        <v>1513561248436.21</v>
+        <v>1629296032639.72</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="1" t="n">
-        <v>0.9676</v>
+        <v>1.001</v>
       </c>
       <c r="B318" s="0" t="n">
-        <v>1629296032639.72</v>
+        <v>1803017740859.57</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="1" t="n">
-        <v>1.001</v>
+        <v>1.0343</v>
       </c>
       <c r="B319" s="0" t="n">
-        <v>1803017740859.57</v>
+        <v>1905460717963.24</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="1" t="n">
-        <v>1.0343</v>
+        <v>1.0677</v>
       </c>
       <c r="B320" s="0" t="n">
-        <v>1905460717963.24</v>
+        <v>2108628149933.29</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="1" t="n">
-        <v>1.0677</v>
+        <v>1.1011</v>
       </c>
       <c r="B321" s="0" t="n">
-        <v>2108628149933.29</v>
+        <v>2488857318282.39</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="1" t="n">
-        <v>1.1011</v>
+        <v>1.1287</v>
       </c>
       <c r="B322" s="0" t="n">
-        <v>2488857318282.39</v>
+        <v>2814232667467.63</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="1" t="n">
-        <v>1.1287</v>
+        <v>1.26</v>
       </c>
       <c r="B323" s="0" t="n">
-        <v>2814232667467.63</v>
+        <v>851843865095.912</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="1" t="n">
-        <v>1.26</v>
+        <v>1.3914</v>
       </c>
       <c r="B324" s="0" t="n">
-        <v>851843865095.912</v>
+        <v>228918030082.122</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="1" t="n">
-        <v>1.3914</v>
+        <v>1.5227</v>
       </c>
       <c r="B325" s="0" t="n">
-        <v>228918030082.122</v>
+        <v>90581602579.5404</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="1" t="n">
-        <v>1.5227</v>
+        <v>1.654</v>
       </c>
       <c r="B326" s="0" t="n">
-        <v>90581602579.5404</v>
+        <v>64773893069.5637</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="1" t="n">
-        <v>1.654</v>
+        <v>1.7854</v>
       </c>
       <c r="B327" s="0" t="n">
-        <v>64773893069.5637</v>
+        <v>53822020832.021</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="1" t="n">
-        <v>1.7854</v>
+        <v>1.9167</v>
       </c>
       <c r="B328" s="0" t="n">
-        <v>53822020832.021</v>
+        <v>48968860708.4891</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="1" t="n">
-        <v>1.9167</v>
+        <v>2.048</v>
       </c>
       <c r="B329" s="0" t="n">
-        <v>48968860708.4891</v>
+        <v>44446748942.7453</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="1" t="n">
-        <v>2.048</v>
+        <v>2.1794</v>
       </c>
       <c r="B330" s="0" t="n">
-        <v>44446748942.7453</v>
+        <v>37635700169.3673</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="1" t="n">
-        <v>2.1794</v>
+        <v>2.3107</v>
       </c>
       <c r="B331" s="0" t="n">
-        <v>37635700169.3673</v>
+        <v>33632565758.3965</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="1" t="n">
-        <v>2.3107</v>
+        <v>2.442</v>
       </c>
       <c r="B332" s="0" t="n">
-        <v>33632565758.3965</v>
+        <v>32427987728.6344</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="1" t="n">
-        <v>2.442</v>
+        <v>2.5734</v>
       </c>
       <c r="B333" s="0" t="n">
-        <v>32427987728.6344</v>
+        <v>32445913049.4009</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="1" t="n">
-        <v>2.5734</v>
+        <v>2.7047</v>
       </c>
       <c r="B334" s="0" t="n">
-        <v>32445913049.4009</v>
+        <v>31783374121.4622</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="1" t="n">
-        <v>2.7047</v>
+        <v>2.836</v>
       </c>
       <c r="B335" s="0" t="n">
-        <v>31783374121.4622</v>
+        <v>31180279221.0286</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="1" t="n">
-        <v>2.836</v>
+        <v>2.9674</v>
       </c>
       <c r="B336" s="0" t="n">
-        <v>31180279221.0286</v>
+        <v>30397649285.7372</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="1" t="n">
-        <v>2.9674</v>
+        <v>3.0987</v>
       </c>
       <c r="B337" s="0" t="n">
-        <v>30397649285.7372</v>
+        <v>29287344787.1636</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="1" t="n">
-        <v>3.0987</v>
+        <v>3.23</v>
       </c>
       <c r="B338" s="0" t="n">
-        <v>29287344787.1636</v>
+        <v>28557487804.4459</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="1" t="n">
-        <v>3.23</v>
+        <v>3.3614</v>
       </c>
       <c r="B339" s="0" t="n">
-        <v>28557487804.4459</v>
+        <v>28183829312.6445</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="1" t="n">
-        <v>3.3614</v>
+        <v>3.4927</v>
       </c>
       <c r="B340" s="0" t="n">
-        <v>28183829312.6445</v>
-      </c>
-    </row>
-    <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A341" s="1" t="n">
-        <v>3.4927</v>
-      </c>
-      <c r="B341" s="0" t="n">
         <v>27792012728.1056</v>
       </c>
     </row>

</xml_diff>